<commit_message>
UPDATing Tasks list for presentation
</commit_message>
<xml_diff>
--- a/PROJECT DOCUMENTATION/FinalProjectGuide.xlsx
+++ b/PROJECT DOCUMENTATION/FinalProjectGuide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Documents\GitHub\FinalProject-MachineLearning\PROJECT DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B41F680-36E3-4A67-987E-033E59D24974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7252D730-667C-4427-B512-F73C98385597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2415" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="11" activeTab="11" xr2:uid="{9D2C2162-F178-4CB0-81E9-DFAA2C429D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -2318,8 +2318,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2339,13 +2346,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3265,7 +3265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959D3522-FC75-4906-B3D0-8D1583483329}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -3371,7 +3371,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3577,7 +3577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E40527A-97EA-4263-8207-1A98E6851C6C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -3626,76 +3626,76 @@
       <c r="B2" s="19"/>
     </row>
     <row r="3" spans="1:489" ht="15.75" thickBot="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="73" t="s">
+      <c r="G3" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="73" t="s">
+      <c r="P3" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="73" t="s">
+      <c r="Q3" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="73" t="s">
+      <c r="R3" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="73" t="s">
+      <c r="S3" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="73" t="s">
+      <c r="T3" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="72" t="s">
+      <c r="U3" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
     </row>
     <row r="4" spans="1:489" ht="30.95" customHeight="1" thickBot="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="A4" s="79"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
       <c r="K4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3709,11 +3709,11 @@
         <v>99</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
       <c r="U4" s="4" t="s">
         <v>96</v>
       </c>
@@ -3825,848 +3825,848 @@
     </row>
     <row r="7" spans="1:489" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A8" s="77"/>
-      <c r="B8" s="75" t="s">
+      <c r="A8" s="80"/>
+      <c r="B8" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="73" t="s">
+      <c r="E8" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I8" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72" t="s">
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72" t="s">
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="T8" s="72" t="s">
+      <c r="T8" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72" t="s">
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="72" t="s">
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72" t="s">
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="72" t="s">
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="AE8" s="72" t="s">
+      <c r="AE8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="AF8" s="72"/>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72" t="s">
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="72" t="s">
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="AL8" s="72"/>
-      <c r="AM8" s="72"/>
-      <c r="AN8" s="72" t="s">
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="AO8" s="72" t="s">
+      <c r="AO8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72"/>
-      <c r="AR8" s="72"/>
-      <c r="AS8" s="72" t="s">
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="AT8" s="72"/>
-      <c r="AU8" s="72"/>
-      <c r="AV8" s="72"/>
-      <c r="AW8" s="72"/>
-      <c r="AX8" s="72" t="s">
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="AY8" s="72"/>
-      <c r="AZ8" s="72"/>
-      <c r="BA8" s="72"/>
-      <c r="BB8" s="72" t="s">
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="BC8" s="72" t="s">
+      <c r="BC8" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="BD8" s="72"/>
-      <c r="BE8" s="72"/>
-      <c r="BF8" s="72" t="s">
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="BG8" s="72"/>
-      <c r="BH8" s="72" t="s">
+      <c r="BG8" s="74"/>
+      <c r="BH8" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="BI8" s="72"/>
-      <c r="BJ8" s="72" t="s">
+      <c r="BI8" s="74"/>
+      <c r="BJ8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="BK8" s="72"/>
-      <c r="BL8" s="72"/>
-      <c r="BM8" s="72" t="s">
+      <c r="BK8" s="74"/>
+      <c r="BL8" s="74"/>
+      <c r="BM8" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="BN8" s="72" t="s">
+      <c r="BN8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="BO8" s="72"/>
-      <c r="BP8" s="72"/>
-      <c r="BQ8" s="72"/>
-      <c r="BR8" s="72" t="s">
+      <c r="BO8" s="74"/>
+      <c r="BP8" s="74"/>
+      <c r="BQ8" s="74"/>
+      <c r="BR8" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="BS8" s="72"/>
-      <c r="BT8" s="72"/>
-      <c r="BU8" s="72"/>
-      <c r="BV8" s="72"/>
-      <c r="BW8" s="72" t="s">
+      <c r="BS8" s="74"/>
+      <c r="BT8" s="74"/>
+      <c r="BU8" s="74"/>
+      <c r="BV8" s="74"/>
+      <c r="BW8" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="BX8" s="72"/>
-      <c r="BY8" s="72"/>
-      <c r="BZ8" s="72"/>
-      <c r="CA8" s="72" t="s">
+      <c r="BX8" s="74"/>
+      <c r="BY8" s="74"/>
+      <c r="BZ8" s="74"/>
+      <c r="CA8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="CB8" s="72" t="s">
+      <c r="CB8" s="74" t="s">
         <v>125</v>
       </c>
-      <c r="CC8" s="72"/>
-      <c r="CD8" s="72"/>
-      <c r="CE8" s="72" t="s">
+      <c r="CC8" s="74"/>
+      <c r="CD8" s="74"/>
+      <c r="CE8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="CF8" s="72"/>
-      <c r="CG8" s="72" t="s">
+      <c r="CF8" s="74"/>
+      <c r="CG8" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="CH8" s="72"/>
-      <c r="CI8" s="72" t="s">
+      <c r="CH8" s="74"/>
+      <c r="CI8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="CJ8" s="72"/>
-      <c r="CK8" s="72"/>
-      <c r="CL8" s="72" t="s">
+      <c r="CJ8" s="74"/>
+      <c r="CK8" s="74"/>
+      <c r="CL8" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="CM8" s="72" t="s">
+      <c r="CM8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="CN8" s="72"/>
-      <c r="CO8" s="72"/>
-      <c r="CP8" s="72"/>
-      <c r="CQ8" s="72" t="s">
+      <c r="CN8" s="74"/>
+      <c r="CO8" s="74"/>
+      <c r="CP8" s="74"/>
+      <c r="CQ8" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="CR8" s="72"/>
-      <c r="CS8" s="72"/>
-      <c r="CT8" s="72"/>
-      <c r="CU8" s="72"/>
-      <c r="CV8" s="72" t="s">
+      <c r="CR8" s="74"/>
+      <c r="CS8" s="74"/>
+      <c r="CT8" s="74"/>
+      <c r="CU8" s="74"/>
+      <c r="CV8" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="CW8" s="72"/>
-      <c r="CX8" s="72"/>
-      <c r="CY8" s="72"/>
-      <c r="CZ8" s="72" t="s">
+      <c r="CW8" s="74"/>
+      <c r="CX8" s="74"/>
+      <c r="CY8" s="74"/>
+      <c r="CZ8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="DA8" s="72" t="s">
+      <c r="DA8" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="DB8" s="72"/>
-      <c r="DC8" s="72"/>
-      <c r="DD8" s="72" t="s">
+      <c r="DB8" s="74"/>
+      <c r="DC8" s="74"/>
+      <c r="DD8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="DE8" s="72"/>
-      <c r="DF8" s="72" t="s">
+      <c r="DE8" s="74"/>
+      <c r="DF8" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="DG8" s="72"/>
-      <c r="DH8" s="72" t="s">
+      <c r="DG8" s="74"/>
+      <c r="DH8" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="DI8" s="72"/>
-      <c r="DJ8" s="72"/>
-      <c r="DK8" s="72" t="s">
+      <c r="DI8" s="74"/>
+      <c r="DJ8" s="74"/>
+      <c r="DK8" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="DL8" s="72" t="s">
+      <c r="DL8" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="DM8" s="72"/>
-      <c r="DN8" s="72"/>
-      <c r="DO8" s="72"/>
-      <c r="DP8" s="72" t="s">
+      <c r="DM8" s="74"/>
+      <c r="DN8" s="74"/>
+      <c r="DO8" s="74"/>
+      <c r="DP8" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="DQ8" s="72"/>
-      <c r="DR8" s="72"/>
-      <c r="DS8" s="72"/>
-      <c r="DT8" s="72"/>
-      <c r="DU8" s="72" t="s">
+      <c r="DQ8" s="74"/>
+      <c r="DR8" s="74"/>
+      <c r="DS8" s="74"/>
+      <c r="DT8" s="74"/>
+      <c r="DU8" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="DV8" s="72"/>
-      <c r="DW8" s="72"/>
-      <c r="DX8" s="72"/>
-      <c r="DY8" s="72" t="s">
+      <c r="DV8" s="74"/>
+      <c r="DW8" s="74"/>
+      <c r="DX8" s="74"/>
+      <c r="DY8" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="DZ8" s="72" t="s">
+      <c r="DZ8" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="EA8" s="72"/>
-      <c r="EB8" s="72"/>
-      <c r="EC8" s="72" t="s">
+      <c r="EA8" s="74"/>
+      <c r="EB8" s="74"/>
+      <c r="EC8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="ED8" s="72"/>
-      <c r="EE8" s="72"/>
-      <c r="EF8" s="72" t="s">
+      <c r="ED8" s="74"/>
+      <c r="EE8" s="74"/>
+      <c r="EF8" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="EG8" s="72"/>
-      <c r="EH8" s="72"/>
-      <c r="EI8" s="72" t="s">
+      <c r="EG8" s="74"/>
+      <c r="EH8" s="74"/>
+      <c r="EI8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="EJ8" s="72"/>
-      <c r="EK8" s="72"/>
-      <c r="EL8" s="72" t="s">
+      <c r="EJ8" s="74"/>
+      <c r="EK8" s="74"/>
+      <c r="EL8" s="74" t="s">
         <v>137</v>
       </c>
-      <c r="EM8" s="72"/>
-      <c r="EN8" s="72"/>
-      <c r="EO8" s="72" t="s">
+      <c r="EM8" s="74"/>
+      <c r="EN8" s="74"/>
+      <c r="EO8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="EP8" s="72"/>
-      <c r="EQ8" s="72"/>
-      <c r="ER8" s="72" t="s">
+      <c r="EP8" s="74"/>
+      <c r="EQ8" s="74"/>
+      <c r="ER8" s="74" t="s">
         <v>138</v>
       </c>
-      <c r="ES8" s="72"/>
-      <c r="ET8" s="72"/>
-      <c r="EU8" s="72" t="s">
+      <c r="ES8" s="74"/>
+      <c r="ET8" s="74"/>
+      <c r="EU8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="EV8" s="72"/>
-      <c r="EW8" s="72"/>
-      <c r="EX8" s="72" t="s">
+      <c r="EV8" s="74"/>
+      <c r="EW8" s="74"/>
+      <c r="EX8" s="74" t="s">
         <v>139</v>
       </c>
-      <c r="EY8" s="72"/>
-      <c r="EZ8" s="72"/>
-      <c r="FA8" s="72" t="s">
+      <c r="EY8" s="74"/>
+      <c r="EZ8" s="74"/>
+      <c r="FA8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="FB8" s="72"/>
-      <c r="FC8" s="72"/>
-      <c r="FD8" s="72" t="s">
+      <c r="FB8" s="74"/>
+      <c r="FC8" s="74"/>
+      <c r="FD8" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="FE8" s="72"/>
-      <c r="FF8" s="72"/>
-      <c r="FG8" s="72" t="s">
+      <c r="FE8" s="74"/>
+      <c r="FF8" s="74"/>
+      <c r="FG8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="FH8" s="72"/>
-      <c r="FI8" s="72"/>
-      <c r="FJ8" s="72" t="s">
+      <c r="FH8" s="74"/>
+      <c r="FI8" s="74"/>
+      <c r="FJ8" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="FK8" s="72"/>
-      <c r="FL8" s="72"/>
-      <c r="FM8" s="72" t="s">
+      <c r="FK8" s="74"/>
+      <c r="FL8" s="74"/>
+      <c r="FM8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="FN8" s="72"/>
-      <c r="FO8" s="72"/>
-      <c r="FP8" s="72" t="s">
+      <c r="FN8" s="74"/>
+      <c r="FO8" s="74"/>
+      <c r="FP8" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="FQ8" s="72"/>
-      <c r="FR8" s="72"/>
-      <c r="FS8" s="72" t="s">
+      <c r="FQ8" s="74"/>
+      <c r="FR8" s="74"/>
+      <c r="FS8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="FT8" s="72"/>
-      <c r="FU8" s="72"/>
-      <c r="FV8" s="72" t="s">
+      <c r="FT8" s="74"/>
+      <c r="FU8" s="74"/>
+      <c r="FV8" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="FW8" s="72"/>
-      <c r="FX8" s="72"/>
-      <c r="FY8" s="72" t="s">
+      <c r="FW8" s="74"/>
+      <c r="FX8" s="74"/>
+      <c r="FY8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="FZ8" s="72"/>
-      <c r="GA8" s="72"/>
-      <c r="GB8" s="72" t="s">
+      <c r="FZ8" s="74"/>
+      <c r="GA8" s="74"/>
+      <c r="GB8" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="GC8" s="72"/>
-      <c r="GD8" s="72"/>
-      <c r="GE8" s="72" t="s">
+      <c r="GC8" s="74"/>
+      <c r="GD8" s="74"/>
+      <c r="GE8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="GF8" s="72"/>
-      <c r="GG8" s="72"/>
-      <c r="GH8" s="72" t="s">
+      <c r="GF8" s="74"/>
+      <c r="GG8" s="74"/>
+      <c r="GH8" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="GI8" s="72"/>
-      <c r="GJ8" s="72"/>
-      <c r="GK8" s="72" t="s">
+      <c r="GI8" s="74"/>
+      <c r="GJ8" s="74"/>
+      <c r="GK8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="GL8" s="72"/>
-      <c r="GM8" s="72"/>
-      <c r="GN8" s="72" t="s">
+      <c r="GL8" s="74"/>
+      <c r="GM8" s="74"/>
+      <c r="GN8" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="GO8" s="72"/>
-      <c r="GP8" s="72"/>
-      <c r="GQ8" s="72" t="s">
+      <c r="GO8" s="74"/>
+      <c r="GP8" s="74"/>
+      <c r="GQ8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="GR8" s="72"/>
-      <c r="GS8" s="72"/>
-      <c r="GT8" s="72" t="s">
+      <c r="GR8" s="74"/>
+      <c r="GS8" s="74"/>
+      <c r="GT8" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="GU8" s="72"/>
-      <c r="GV8" s="72"/>
-      <c r="GW8" s="72" t="s">
+      <c r="GU8" s="74"/>
+      <c r="GV8" s="74"/>
+      <c r="GW8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="GX8" s="72"/>
-      <c r="GY8" s="72"/>
-      <c r="GZ8" s="72" t="s">
+      <c r="GX8" s="74"/>
+      <c r="GY8" s="74"/>
+      <c r="GZ8" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="HA8" s="72"/>
-      <c r="HB8" s="72"/>
-      <c r="HC8" s="72" t="s">
+      <c r="HA8" s="74"/>
+      <c r="HB8" s="74"/>
+      <c r="HC8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="HD8" s="72"/>
-      <c r="HE8" s="72"/>
-      <c r="HF8" s="72" t="s">
+      <c r="HD8" s="74"/>
+      <c r="HE8" s="74"/>
+      <c r="HF8" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="HG8" s="72"/>
-      <c r="HH8" s="72"/>
-      <c r="HI8" s="72" t="s">
+      <c r="HG8" s="74"/>
+      <c r="HH8" s="74"/>
+      <c r="HI8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="HJ8" s="72"/>
-      <c r="HK8" s="72"/>
-      <c r="HL8" s="72" t="s">
+      <c r="HJ8" s="74"/>
+      <c r="HK8" s="74"/>
+      <c r="HL8" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="HM8" s="72"/>
-      <c r="HN8" s="72"/>
-      <c r="HO8" s="72" t="s">
+      <c r="HM8" s="74"/>
+      <c r="HN8" s="74"/>
+      <c r="HO8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="HP8" s="72"/>
-      <c r="HQ8" s="72"/>
-      <c r="HR8" s="72" t="s">
+      <c r="HP8" s="74"/>
+      <c r="HQ8" s="74"/>
+      <c r="HR8" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="HS8" s="72"/>
-      <c r="HT8" s="72"/>
-      <c r="HU8" s="72" t="s">
+      <c r="HS8" s="74"/>
+      <c r="HT8" s="74"/>
+      <c r="HU8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="HV8" s="72"/>
-      <c r="HW8" s="72"/>
-      <c r="HX8" s="72" t="s">
+      <c r="HV8" s="74"/>
+      <c r="HW8" s="74"/>
+      <c r="HX8" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="HY8" s="72"/>
-      <c r="HZ8" s="72"/>
-      <c r="IA8" s="72" t="s">
+      <c r="HY8" s="74"/>
+      <c r="HZ8" s="74"/>
+      <c r="IA8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="IB8" s="72"/>
-      <c r="IC8" s="72"/>
-      <c r="ID8" s="72" t="s">
+      <c r="IB8" s="74"/>
+      <c r="IC8" s="74"/>
+      <c r="ID8" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="IE8" s="72"/>
-      <c r="IF8" s="72"/>
-      <c r="IG8" s="72" t="s">
+      <c r="IE8" s="74"/>
+      <c r="IF8" s="74"/>
+      <c r="IG8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="IH8" s="72"/>
-      <c r="II8" s="72"/>
-      <c r="IJ8" s="72" t="s">
+      <c r="IH8" s="74"/>
+      <c r="II8" s="74"/>
+      <c r="IJ8" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="IK8" s="72"/>
-      <c r="IL8" s="72"/>
-      <c r="IM8" s="72" t="s">
+      <c r="IK8" s="74"/>
+      <c r="IL8" s="74"/>
+      <c r="IM8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="IN8" s="72"/>
-      <c r="IO8" s="72"/>
-      <c r="IP8" s="72" t="s">
+      <c r="IN8" s="74"/>
+      <c r="IO8" s="74"/>
+      <c r="IP8" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="IQ8" s="72"/>
-      <c r="IR8" s="72"/>
-      <c r="IS8" s="72" t="s">
+      <c r="IQ8" s="74"/>
+      <c r="IR8" s="74"/>
+      <c r="IS8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="IT8" s="72"/>
-      <c r="IU8" s="72"/>
-      <c r="IV8" s="72" t="s">
+      <c r="IT8" s="74"/>
+      <c r="IU8" s="74"/>
+      <c r="IV8" s="74" t="s">
         <v>156</v>
       </c>
-      <c r="IW8" s="72"/>
-      <c r="IX8" s="72"/>
-      <c r="IY8" s="72" t="s">
+      <c r="IW8" s="74"/>
+      <c r="IX8" s="74"/>
+      <c r="IY8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="IZ8" s="72"/>
-      <c r="JA8" s="72"/>
-      <c r="JB8" s="72" t="s">
+      <c r="IZ8" s="74"/>
+      <c r="JA8" s="74"/>
+      <c r="JB8" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="JC8" s="72"/>
-      <c r="JD8" s="72"/>
-      <c r="JE8" s="72" t="s">
+      <c r="JC8" s="74"/>
+      <c r="JD8" s="74"/>
+      <c r="JE8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="JF8" s="72"/>
-      <c r="JG8" s="72"/>
-      <c r="JH8" s="72" t="s">
+      <c r="JF8" s="74"/>
+      <c r="JG8" s="74"/>
+      <c r="JH8" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="JI8" s="72"/>
-      <c r="JJ8" s="72"/>
-      <c r="JK8" s="72" t="s">
+      <c r="JI8" s="74"/>
+      <c r="JJ8" s="74"/>
+      <c r="JK8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="JL8" s="72"/>
-      <c r="JM8" s="72"/>
-      <c r="JN8" s="72" t="s">
+      <c r="JL8" s="74"/>
+      <c r="JM8" s="74"/>
+      <c r="JN8" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="JO8" s="72"/>
-      <c r="JP8" s="72"/>
-      <c r="JQ8" s="72" t="s">
+      <c r="JO8" s="74"/>
+      <c r="JP8" s="74"/>
+      <c r="JQ8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="JR8" s="72"/>
-      <c r="JS8" s="72"/>
-      <c r="JT8" s="72" t="s">
+      <c r="JR8" s="74"/>
+      <c r="JS8" s="74"/>
+      <c r="JT8" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="JU8" s="72"/>
-      <c r="JV8" s="72"/>
-      <c r="JW8" s="72" t="s">
+      <c r="JU8" s="74"/>
+      <c r="JV8" s="74"/>
+      <c r="JW8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="JX8" s="72"/>
-      <c r="JY8" s="72"/>
-      <c r="JZ8" s="72" t="s">
+      <c r="JX8" s="74"/>
+      <c r="JY8" s="74"/>
+      <c r="JZ8" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="KA8" s="72"/>
-      <c r="KB8" s="72"/>
-      <c r="KC8" s="72" t="s">
+      <c r="KA8" s="74"/>
+      <c r="KB8" s="74"/>
+      <c r="KC8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="KD8" s="72"/>
-      <c r="KE8" s="72"/>
-      <c r="KF8" s="72" t="s">
+      <c r="KD8" s="74"/>
+      <c r="KE8" s="74"/>
+      <c r="KF8" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="KG8" s="72"/>
-      <c r="KH8" s="72"/>
-      <c r="KI8" s="72" t="s">
+      <c r="KG8" s="74"/>
+      <c r="KH8" s="74"/>
+      <c r="KI8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="KJ8" s="72"/>
-      <c r="KK8" s="72"/>
-      <c r="KL8" s="72" t="s">
+      <c r="KJ8" s="74"/>
+      <c r="KK8" s="74"/>
+      <c r="KL8" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="KM8" s="72"/>
-      <c r="KN8" s="72"/>
-      <c r="KO8" s="72" t="s">
+      <c r="KM8" s="74"/>
+      <c r="KN8" s="74"/>
+      <c r="KO8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="KP8" s="72"/>
-      <c r="KQ8" s="72"/>
-      <c r="KR8" s="72" t="s">
+      <c r="KP8" s="74"/>
+      <c r="KQ8" s="74"/>
+      <c r="KR8" s="74" t="s">
         <v>164</v>
       </c>
-      <c r="KS8" s="72"/>
-      <c r="KT8" s="72"/>
-      <c r="KU8" s="72" t="s">
+      <c r="KS8" s="74"/>
+      <c r="KT8" s="74"/>
+      <c r="KU8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="KV8" s="72"/>
-      <c r="KW8" s="72"/>
-      <c r="KX8" s="72" t="s">
+      <c r="KV8" s="74"/>
+      <c r="KW8" s="74"/>
+      <c r="KX8" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="KY8" s="72"/>
-      <c r="KZ8" s="72"/>
-      <c r="LA8" s="72" t="s">
+      <c r="KY8" s="74"/>
+      <c r="KZ8" s="74"/>
+      <c r="LA8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="LB8" s="72"/>
-      <c r="LC8" s="72"/>
-      <c r="LD8" s="72" t="s">
+      <c r="LB8" s="74"/>
+      <c r="LC8" s="74"/>
+      <c r="LD8" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="LE8" s="72"/>
-      <c r="LF8" s="72"/>
-      <c r="LG8" s="72" t="s">
+      <c r="LE8" s="74"/>
+      <c r="LF8" s="74"/>
+      <c r="LG8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="LH8" s="72"/>
-      <c r="LI8" s="72"/>
-      <c r="LJ8" s="72" t="s">
+      <c r="LH8" s="74"/>
+      <c r="LI8" s="74"/>
+      <c r="LJ8" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="LK8" s="72"/>
-      <c r="LL8" s="72"/>
-      <c r="LM8" s="72" t="s">
+      <c r="LK8" s="74"/>
+      <c r="LL8" s="74"/>
+      <c r="LM8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="LN8" s="72"/>
-      <c r="LO8" s="72"/>
-      <c r="LP8" s="72" t="s">
+      <c r="LN8" s="74"/>
+      <c r="LO8" s="74"/>
+      <c r="LP8" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="LQ8" s="72"/>
-      <c r="LR8" s="72"/>
-      <c r="LS8" s="72" t="s">
+      <c r="LQ8" s="74"/>
+      <c r="LR8" s="74"/>
+      <c r="LS8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="LT8" s="72"/>
-      <c r="LU8" s="72"/>
-      <c r="LV8" s="72" t="s">
+      <c r="LT8" s="74"/>
+      <c r="LU8" s="74"/>
+      <c r="LV8" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="LW8" s="72"/>
-      <c r="LX8" s="72"/>
-      <c r="LY8" s="72" t="s">
+      <c r="LW8" s="74"/>
+      <c r="LX8" s="74"/>
+      <c r="LY8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="LZ8" s="72"/>
-      <c r="MA8" s="72"/>
-      <c r="MB8" s="72" t="s">
+      <c r="LZ8" s="74"/>
+      <c r="MA8" s="74"/>
+      <c r="MB8" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="MC8" s="72"/>
-      <c r="MD8" s="72"/>
-      <c r="ME8" s="72" t="s">
+      <c r="MC8" s="74"/>
+      <c r="MD8" s="74"/>
+      <c r="ME8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="MF8" s="72"/>
-      <c r="MG8" s="72"/>
-      <c r="MH8" s="72" t="s">
+      <c r="MF8" s="74"/>
+      <c r="MG8" s="74"/>
+      <c r="MH8" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="MI8" s="72"/>
-      <c r="MJ8" s="72"/>
-      <c r="MK8" s="72" t="s">
+      <c r="MI8" s="74"/>
+      <c r="MJ8" s="74"/>
+      <c r="MK8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="ML8" s="72"/>
-      <c r="MM8" s="72"/>
-      <c r="MN8" s="72" t="s">
+      <c r="ML8" s="74"/>
+      <c r="MM8" s="74"/>
+      <c r="MN8" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="MO8" s="72"/>
-      <c r="MP8" s="72"/>
-      <c r="MQ8" s="72" t="s">
+      <c r="MO8" s="74"/>
+      <c r="MP8" s="74"/>
+      <c r="MQ8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="MR8" s="72"/>
-      <c r="MS8" s="72"/>
-      <c r="MT8" s="72" t="s">
+      <c r="MR8" s="74"/>
+      <c r="MS8" s="74"/>
+      <c r="MT8" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="MU8" s="72"/>
-      <c r="MV8" s="72"/>
-      <c r="MW8" s="72" t="s">
+      <c r="MU8" s="74"/>
+      <c r="MV8" s="74"/>
+      <c r="MW8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="MX8" s="72"/>
-      <c r="MY8" s="72"/>
-      <c r="MZ8" s="72" t="s">
+      <c r="MX8" s="74"/>
+      <c r="MY8" s="74"/>
+      <c r="MZ8" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="NA8" s="72"/>
-      <c r="NB8" s="72"/>
-      <c r="NC8" s="72" t="s">
+      <c r="NA8" s="74"/>
+      <c r="NB8" s="74"/>
+      <c r="NC8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="ND8" s="72"/>
-      <c r="NE8" s="72"/>
-      <c r="NF8" s="72" t="s">
+      <c r="ND8" s="74"/>
+      <c r="NE8" s="74"/>
+      <c r="NF8" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="NG8" s="72"/>
-      <c r="NH8" s="72"/>
-      <c r="NI8" s="72" t="s">
+      <c r="NG8" s="74"/>
+      <c r="NH8" s="74"/>
+      <c r="NI8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="NJ8" s="72"/>
-      <c r="NK8" s="72"/>
-      <c r="NL8" s="72" t="s">
+      <c r="NJ8" s="74"/>
+      <c r="NK8" s="74"/>
+      <c r="NL8" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="NM8" s="72"/>
-      <c r="NN8" s="72"/>
-      <c r="NO8" s="72" t="s">
+      <c r="NM8" s="74"/>
+      <c r="NN8" s="74"/>
+      <c r="NO8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="NP8" s="72"/>
-      <c r="NQ8" s="72"/>
-      <c r="NR8" s="72" t="s">
+      <c r="NP8" s="74"/>
+      <c r="NQ8" s="74"/>
+      <c r="NR8" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="NS8" s="72"/>
-      <c r="NT8" s="72"/>
-      <c r="NU8" s="72" t="s">
+      <c r="NS8" s="74"/>
+      <c r="NT8" s="74"/>
+      <c r="NU8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="NV8" s="72"/>
-      <c r="NW8" s="72"/>
-      <c r="NX8" s="72" t="s">
+      <c r="NV8" s="74"/>
+      <c r="NW8" s="74"/>
+      <c r="NX8" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="NY8" s="72"/>
-      <c r="NZ8" s="72"/>
-      <c r="OA8" s="72" t="s">
+      <c r="NY8" s="74"/>
+      <c r="NZ8" s="74"/>
+      <c r="OA8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="OB8" s="72"/>
-      <c r="OC8" s="72"/>
-      <c r="OD8" s="72" t="s">
+      <c r="OB8" s="74"/>
+      <c r="OC8" s="74"/>
+      <c r="OD8" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="OE8" s="72"/>
-      <c r="OF8" s="72"/>
-      <c r="OG8" s="72" t="s">
+      <c r="OE8" s="74"/>
+      <c r="OF8" s="74"/>
+      <c r="OG8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="OH8" s="72"/>
-      <c r="OI8" s="72"/>
-      <c r="OJ8" s="72" t="s">
+      <c r="OH8" s="74"/>
+      <c r="OI8" s="74"/>
+      <c r="OJ8" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="OK8" s="72"/>
-      <c r="OL8" s="72"/>
-      <c r="OM8" s="72" t="s">
+      <c r="OK8" s="74"/>
+      <c r="OL8" s="74"/>
+      <c r="OM8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="ON8" s="72"/>
-      <c r="OO8" s="72"/>
-      <c r="OP8" s="72" t="s">
+      <c r="ON8" s="74"/>
+      <c r="OO8" s="74"/>
+      <c r="OP8" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="OQ8" s="72"/>
-      <c r="OR8" s="72"/>
-      <c r="OS8" s="72" t="s">
+      <c r="OQ8" s="74"/>
+      <c r="OR8" s="74"/>
+      <c r="OS8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="OT8" s="72"/>
-      <c r="OU8" s="72"/>
-      <c r="OV8" s="72" t="s">
+      <c r="OT8" s="74"/>
+      <c r="OU8" s="74"/>
+      <c r="OV8" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="OW8" s="72"/>
-      <c r="OX8" s="72"/>
-      <c r="OY8" s="72" t="s">
+      <c r="OW8" s="74"/>
+      <c r="OX8" s="74"/>
+      <c r="OY8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="OZ8" s="72"/>
-      <c r="PA8" s="72"/>
-      <c r="PB8" s="72" t="s">
+      <c r="OZ8" s="74"/>
+      <c r="PA8" s="74"/>
+      <c r="PB8" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="PC8" s="72"/>
-      <c r="PD8" s="72"/>
-      <c r="PE8" s="72" t="s">
+      <c r="PC8" s="74"/>
+      <c r="PD8" s="74"/>
+      <c r="PE8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="PF8" s="72"/>
-      <c r="PG8" s="72"/>
-      <c r="PH8" s="72" t="s">
+      <c r="PF8" s="74"/>
+      <c r="PG8" s="74"/>
+      <c r="PH8" s="74" t="s">
         <v>184</v>
       </c>
-      <c r="PI8" s="72"/>
-      <c r="PJ8" s="72"/>
-      <c r="PK8" s="72" t="s">
+      <c r="PI8" s="74"/>
+      <c r="PJ8" s="74"/>
+      <c r="PK8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="PL8" s="72"/>
-      <c r="PM8" s="72"/>
-      <c r="PN8" s="72" t="s">
+      <c r="PL8" s="74"/>
+      <c r="PM8" s="74"/>
+      <c r="PN8" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="PO8" s="72"/>
-      <c r="PP8" s="72"/>
-      <c r="PQ8" s="72" t="s">
+      <c r="PO8" s="74"/>
+      <c r="PP8" s="74"/>
+      <c r="PQ8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="PR8" s="72"/>
-      <c r="PS8" s="72"/>
-      <c r="PT8" s="72" t="s">
+      <c r="PR8" s="74"/>
+      <c r="PS8" s="74"/>
+      <c r="PT8" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="PU8" s="72"/>
-      <c r="PV8" s="72"/>
-      <c r="PW8" s="72" t="s">
+      <c r="PU8" s="74"/>
+      <c r="PV8" s="74"/>
+      <c r="PW8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="PX8" s="72"/>
-      <c r="PY8" s="72"/>
-      <c r="PZ8" s="72" t="s">
+      <c r="PX8" s="74"/>
+      <c r="PY8" s="74"/>
+      <c r="PZ8" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="QA8" s="72"/>
-      <c r="QB8" s="72"/>
-      <c r="QC8" s="72" t="s">
+      <c r="QA8" s="74"/>
+      <c r="QB8" s="74"/>
+      <c r="QC8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="QD8" s="72"/>
-      <c r="QE8" s="72"/>
-      <c r="QF8" s="72" t="s">
+      <c r="QD8" s="74"/>
+      <c r="QE8" s="74"/>
+      <c r="QF8" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="QG8" s="72"/>
-      <c r="QH8" s="72"/>
-      <c r="QI8" s="72" t="s">
+      <c r="QG8" s="74"/>
+      <c r="QH8" s="74"/>
+      <c r="QI8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="QJ8" s="72"/>
-      <c r="QK8" s="72"/>
-      <c r="QL8" s="72" t="s">
+      <c r="QJ8" s="74"/>
+      <c r="QK8" s="74"/>
+      <c r="QL8" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="QM8" s="72"/>
-      <c r="QN8" s="72"/>
-      <c r="QO8" s="72" t="s">
+      <c r="QM8" s="74"/>
+      <c r="QN8" s="74"/>
+      <c r="QO8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="QP8" s="72"/>
-      <c r="QQ8" s="72"/>
-      <c r="QR8" s="72" t="s">
+      <c r="QP8" s="74"/>
+      <c r="QQ8" s="74"/>
+      <c r="QR8" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="QS8" s="72"/>
-      <c r="QT8" s="72"/>
-      <c r="QU8" s="72" t="s">
+      <c r="QS8" s="74"/>
+      <c r="QT8" s="74"/>
+      <c r="QU8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="QV8" s="72"/>
-      <c r="QW8" s="72"/>
-      <c r="QX8" s="72" t="s">
+      <c r="QV8" s="74"/>
+      <c r="QW8" s="74"/>
+      <c r="QX8" s="74" t="s">
         <v>191</v>
       </c>
-      <c r="QY8" s="72"/>
-      <c r="QZ8" s="72"/>
-      <c r="RA8" s="72" t="s">
+      <c r="QY8" s="74"/>
+      <c r="QZ8" s="74"/>
+      <c r="RA8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="RB8" s="72"/>
-      <c r="RC8" s="72"/>
-      <c r="RD8" s="72" t="s">
+      <c r="RB8" s="74"/>
+      <c r="RC8" s="74"/>
+      <c r="RD8" s="74" t="s">
         <v>192</v>
       </c>
-      <c r="RE8" s="72"/>
-      <c r="RF8" s="72"/>
-      <c r="RG8" s="72" t="s">
+      <c r="RE8" s="74"/>
+      <c r="RF8" s="74"/>
+      <c r="RG8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="RH8" s="72"/>
-      <c r="RI8" s="72"/>
-      <c r="RJ8" s="72" t="s">
+      <c r="RH8" s="74"/>
+      <c r="RI8" s="74"/>
+      <c r="RJ8" s="74" t="s">
         <v>193</v>
       </c>
-      <c r="RK8" s="72"/>
-      <c r="RL8" s="72"/>
-      <c r="RM8" s="72" t="s">
+      <c r="RK8" s="74"/>
+      <c r="RL8" s="74"/>
+      <c r="RM8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="RN8" s="72"/>
-      <c r="RO8" s="72"/>
-      <c r="RP8" s="72" t="s">
+      <c r="RN8" s="74"/>
+      <c r="RO8" s="74"/>
+      <c r="RP8" s="74" t="s">
         <v>194</v>
       </c>
-      <c r="RQ8" s="72"/>
-      <c r="RR8" s="72"/>
-      <c r="RS8" s="72" t="s">
+      <c r="RQ8" s="74"/>
+      <c r="RR8" s="74"/>
+      <c r="RS8" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="RT8" s="72"/>
-      <c r="RU8" s="72"/>
+      <c r="RT8" s="74"/>
+      <c r="RU8" s="74"/>
     </row>
     <row r="9" spans="1:489" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="74"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="77"/>
       <c r="J9" s="4" t="s">
         <v>96</v>
       </c>
@@ -7494,39 +7494,39 @@
       </c>
     </row>
     <row r="34" spans="1:78" ht="15" customHeight="1">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="75" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
     </row>
     <row r="35" spans="1:78">
-      <c r="A35" s="79"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="75"/>
     </row>
     <row r="36" spans="1:78" ht="78.75" customHeight="1">
-      <c r="A36" s="79"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="79"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
     </row>
     <row r="38" spans="1:78">
       <c r="A38" s="1" t="s">
@@ -7854,120 +7854,120 @@
     <row r="47" spans="1:78">
       <c r="A47" s="43"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="80">
+      <c r="C47" s="72">
         <v>1998</v>
       </c>
-      <c r="D47" s="81"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="80">
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="72">
         <v>1999</v>
       </c>
-      <c r="H47" s="81"/>
-      <c r="I47" s="81"/>
-      <c r="J47" s="81"/>
-      <c r="K47" s="80">
+      <c r="H47" s="73"/>
+      <c r="I47" s="73"/>
+      <c r="J47" s="73"/>
+      <c r="K47" s="72">
         <v>2000</v>
       </c>
-      <c r="L47" s="81"/>
-      <c r="M47" s="81"/>
-      <c r="N47" s="81"/>
-      <c r="O47" s="80">
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73"/>
+      <c r="O47" s="72">
         <v>2001</v>
       </c>
-      <c r="P47" s="81"/>
-      <c r="Q47" s="81"/>
-      <c r="R47" s="81"/>
-      <c r="S47" s="80">
+      <c r="P47" s="73"/>
+      <c r="Q47" s="73"/>
+      <c r="R47" s="73"/>
+      <c r="S47" s="72">
         <v>2002</v>
       </c>
-      <c r="T47" s="81"/>
-      <c r="U47" s="81"/>
-      <c r="V47" s="81"/>
-      <c r="W47" s="80">
+      <c r="T47" s="73"/>
+      <c r="U47" s="73"/>
+      <c r="V47" s="73"/>
+      <c r="W47" s="72">
         <v>2003</v>
       </c>
-      <c r="X47" s="81"/>
-      <c r="Y47" s="81"/>
-      <c r="Z47" s="81"/>
-      <c r="AA47" s="80">
+      <c r="X47" s="73"/>
+      <c r="Y47" s="73"/>
+      <c r="Z47" s="73"/>
+      <c r="AA47" s="72">
         <v>2004</v>
       </c>
-      <c r="AB47" s="81"/>
-      <c r="AC47" s="81"/>
-      <c r="AD47" s="81"/>
-      <c r="AE47" s="80">
+      <c r="AB47" s="73"/>
+      <c r="AC47" s="73"/>
+      <c r="AD47" s="73"/>
+      <c r="AE47" s="72">
         <v>2005</v>
       </c>
-      <c r="AF47" s="81"/>
-      <c r="AG47" s="81"/>
-      <c r="AH47" s="81"/>
-      <c r="AI47" s="80">
+      <c r="AF47" s="73"/>
+      <c r="AG47" s="73"/>
+      <c r="AH47" s="73"/>
+      <c r="AI47" s="72">
         <v>2006</v>
       </c>
-      <c r="AJ47" s="81"/>
-      <c r="AK47" s="81"/>
-      <c r="AL47" s="81"/>
-      <c r="AM47" s="80">
+      <c r="AJ47" s="73"/>
+      <c r="AK47" s="73"/>
+      <c r="AL47" s="73"/>
+      <c r="AM47" s="72">
         <v>2007</v>
       </c>
-      <c r="AN47" s="81"/>
-      <c r="AO47" s="81"/>
-      <c r="AP47" s="81"/>
-      <c r="AQ47" s="80">
+      <c r="AN47" s="73"/>
+      <c r="AO47" s="73"/>
+      <c r="AP47" s="73"/>
+      <c r="AQ47" s="72">
         <v>2008</v>
       </c>
-      <c r="AR47" s="81"/>
-      <c r="AS47" s="81"/>
-      <c r="AT47" s="81"/>
-      <c r="AU47" s="80">
+      <c r="AR47" s="73"/>
+      <c r="AS47" s="73"/>
+      <c r="AT47" s="73"/>
+      <c r="AU47" s="72">
         <v>2009</v>
       </c>
-      <c r="AV47" s="81"/>
-      <c r="AW47" s="81"/>
-      <c r="AX47" s="81"/>
-      <c r="AY47" s="80">
+      <c r="AV47" s="73"/>
+      <c r="AW47" s="73"/>
+      <c r="AX47" s="73"/>
+      <c r="AY47" s="72">
         <v>2010</v>
       </c>
-      <c r="AZ47" s="81"/>
-      <c r="BA47" s="81"/>
-      <c r="BB47" s="81"/>
-      <c r="BC47" s="80">
+      <c r="AZ47" s="73"/>
+      <c r="BA47" s="73"/>
+      <c r="BB47" s="73"/>
+      <c r="BC47" s="72">
         <v>2011</v>
       </c>
-      <c r="BD47" s="81"/>
-      <c r="BE47" s="81"/>
-      <c r="BF47" s="81"/>
-      <c r="BG47" s="80">
+      <c r="BD47" s="73"/>
+      <c r="BE47" s="73"/>
+      <c r="BF47" s="73"/>
+      <c r="BG47" s="72">
         <v>2012</v>
       </c>
-      <c r="BH47" s="81"/>
-      <c r="BI47" s="81"/>
-      <c r="BJ47" s="81"/>
-      <c r="BK47" s="80">
+      <c r="BH47" s="73"/>
+      <c r="BI47" s="73"/>
+      <c r="BJ47" s="73"/>
+      <c r="BK47" s="72">
         <v>2013</v>
       </c>
-      <c r="BL47" s="81"/>
-      <c r="BM47" s="81"/>
-      <c r="BN47" s="81"/>
-      <c r="BO47" s="80">
+      <c r="BL47" s="73"/>
+      <c r="BM47" s="73"/>
+      <c r="BN47" s="73"/>
+      <c r="BO47" s="72">
         <v>2014</v>
       </c>
-      <c r="BP47" s="81"/>
-      <c r="BQ47" s="81"/>
-      <c r="BR47" s="81"/>
-      <c r="BS47" s="80">
+      <c r="BP47" s="73"/>
+      <c r="BQ47" s="73"/>
+      <c r="BR47" s="73"/>
+      <c r="BS47" s="72">
         <v>2015</v>
       </c>
-      <c r="BT47" s="81"/>
-      <c r="BU47" s="81"/>
-      <c r="BV47" s="81"/>
-      <c r="BW47" s="80">
+      <c r="BT47" s="73"/>
+      <c r="BU47" s="73"/>
+      <c r="BV47" s="73"/>
+      <c r="BW47" s="72">
         <v>2016</v>
       </c>
-      <c r="BX47" s="81"/>
-      <c r="BY47" s="81"/>
-      <c r="BZ47" s="81"/>
+      <c r="BX47" s="73"/>
+      <c r="BY47" s="73"/>
+      <c r="BZ47" s="73"/>
     </row>
     <row r="48" spans="1:78">
       <c r="A48" s="44" t="s">
@@ -14077,25 +14077,93 @@
     </row>
   </sheetData>
   <mergeCells count="130">
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="O47:R47"/>
-    <mergeCell ref="S47:V47"/>
-    <mergeCell ref="W47:Z47"/>
-    <mergeCell ref="AA47:AD47"/>
-    <mergeCell ref="AE47:AH47"/>
-    <mergeCell ref="AI47:AL47"/>
-    <mergeCell ref="AM47:AP47"/>
-    <mergeCell ref="BK47:BN47"/>
-    <mergeCell ref="BO47:BR47"/>
-    <mergeCell ref="BS47:BV47"/>
-    <mergeCell ref="BW47:BZ47"/>
-    <mergeCell ref="AQ47:AT47"/>
-    <mergeCell ref="AU47:AX47"/>
-    <mergeCell ref="AY47:BB47"/>
-    <mergeCell ref="BC47:BF47"/>
-    <mergeCell ref="BG47:BJ47"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AX8:BB8"/>
+    <mergeCell ref="BC8:BG8"/>
+    <mergeCell ref="BH8:BL8"/>
+    <mergeCell ref="BM8:BQ8"/>
+    <mergeCell ref="BR8:BV8"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="BW8:CA8"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="AD8:AH8"/>
+    <mergeCell ref="AI8:AM8"/>
+    <mergeCell ref="AN8:AR8"/>
+    <mergeCell ref="AS8:AW8"/>
+    <mergeCell ref="DF8:DJ8"/>
+    <mergeCell ref="DK8:DO8"/>
+    <mergeCell ref="DP8:DT8"/>
+    <mergeCell ref="DU8:DY8"/>
+    <mergeCell ref="DZ8:EE8"/>
+    <mergeCell ref="EF8:EK8"/>
+    <mergeCell ref="CB8:CF8"/>
+    <mergeCell ref="CG8:CK8"/>
+    <mergeCell ref="CL8:CP8"/>
+    <mergeCell ref="CQ8:CU8"/>
+    <mergeCell ref="CV8:CZ8"/>
+    <mergeCell ref="DA8:DE8"/>
+    <mergeCell ref="FV8:GA8"/>
+    <mergeCell ref="GB8:GG8"/>
+    <mergeCell ref="GH8:GM8"/>
+    <mergeCell ref="GN8:GS8"/>
+    <mergeCell ref="GT8:GY8"/>
+    <mergeCell ref="GZ8:HE8"/>
+    <mergeCell ref="EL8:EQ8"/>
+    <mergeCell ref="ER8:EW8"/>
+    <mergeCell ref="EX8:FC8"/>
+    <mergeCell ref="FD8:FI8"/>
+    <mergeCell ref="FJ8:FO8"/>
+    <mergeCell ref="FP8:FU8"/>
+    <mergeCell ref="IP8:IU8"/>
+    <mergeCell ref="IV8:JA8"/>
+    <mergeCell ref="JB8:JG8"/>
+    <mergeCell ref="JH8:JM8"/>
+    <mergeCell ref="JN8:JS8"/>
+    <mergeCell ref="JT8:JY8"/>
+    <mergeCell ref="HF8:HK8"/>
+    <mergeCell ref="HL8:HQ8"/>
+    <mergeCell ref="HR8:HW8"/>
+    <mergeCell ref="HX8:IC8"/>
+    <mergeCell ref="ID8:II8"/>
+    <mergeCell ref="IJ8:IO8"/>
+    <mergeCell ref="LP8:LU8"/>
+    <mergeCell ref="LV8:MA8"/>
+    <mergeCell ref="MB8:MG8"/>
+    <mergeCell ref="MH8:MM8"/>
+    <mergeCell ref="MN8:MS8"/>
+    <mergeCell ref="JZ8:KE8"/>
+    <mergeCell ref="KF8:KK8"/>
+    <mergeCell ref="KL8:KQ8"/>
+    <mergeCell ref="KR8:KW8"/>
+    <mergeCell ref="KX8:LC8"/>
+    <mergeCell ref="LD8:LI8"/>
     <mergeCell ref="QX8:RC8"/>
     <mergeCell ref="RD8:RI8"/>
     <mergeCell ref="RJ8:RO8"/>
@@ -14120,93 +14188,25 @@
     <mergeCell ref="NR8:NW8"/>
     <mergeCell ref="NX8:OC8"/>
     <mergeCell ref="LJ8:LO8"/>
-    <mergeCell ref="LP8:LU8"/>
-    <mergeCell ref="LV8:MA8"/>
-    <mergeCell ref="MB8:MG8"/>
-    <mergeCell ref="MH8:MM8"/>
-    <mergeCell ref="MN8:MS8"/>
-    <mergeCell ref="JZ8:KE8"/>
-    <mergeCell ref="KF8:KK8"/>
-    <mergeCell ref="KL8:KQ8"/>
-    <mergeCell ref="KR8:KW8"/>
-    <mergeCell ref="KX8:LC8"/>
-    <mergeCell ref="LD8:LI8"/>
-    <mergeCell ref="IP8:IU8"/>
-    <mergeCell ref="IV8:JA8"/>
-    <mergeCell ref="JB8:JG8"/>
-    <mergeCell ref="JH8:JM8"/>
-    <mergeCell ref="JN8:JS8"/>
-    <mergeCell ref="JT8:JY8"/>
-    <mergeCell ref="HF8:HK8"/>
-    <mergeCell ref="HL8:HQ8"/>
-    <mergeCell ref="HR8:HW8"/>
-    <mergeCell ref="HX8:IC8"/>
-    <mergeCell ref="ID8:II8"/>
-    <mergeCell ref="IJ8:IO8"/>
-    <mergeCell ref="FV8:GA8"/>
-    <mergeCell ref="GB8:GG8"/>
-    <mergeCell ref="GH8:GM8"/>
-    <mergeCell ref="GN8:GS8"/>
-    <mergeCell ref="GT8:GY8"/>
-    <mergeCell ref="GZ8:HE8"/>
-    <mergeCell ref="EL8:EQ8"/>
-    <mergeCell ref="ER8:EW8"/>
-    <mergeCell ref="EX8:FC8"/>
-    <mergeCell ref="FD8:FI8"/>
-    <mergeCell ref="FJ8:FO8"/>
-    <mergeCell ref="FP8:FU8"/>
-    <mergeCell ref="DP8:DT8"/>
-    <mergeCell ref="DU8:DY8"/>
-    <mergeCell ref="DZ8:EE8"/>
-    <mergeCell ref="EF8:EK8"/>
-    <mergeCell ref="CB8:CF8"/>
-    <mergeCell ref="CG8:CK8"/>
-    <mergeCell ref="CL8:CP8"/>
-    <mergeCell ref="CQ8:CU8"/>
-    <mergeCell ref="CV8:CZ8"/>
-    <mergeCell ref="DA8:DE8"/>
-    <mergeCell ref="BW8:CA8"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="AD8:AH8"/>
-    <mergeCell ref="AI8:AM8"/>
-    <mergeCell ref="AN8:AR8"/>
-    <mergeCell ref="AS8:AW8"/>
-    <mergeCell ref="DF8:DJ8"/>
-    <mergeCell ref="DK8:DO8"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="AX8:BB8"/>
-    <mergeCell ref="BC8:BG8"/>
-    <mergeCell ref="BH8:BL8"/>
-    <mergeCell ref="BM8:BQ8"/>
-    <mergeCell ref="BR8:BV8"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="AM47:AP47"/>
+    <mergeCell ref="BK47:BN47"/>
+    <mergeCell ref="BO47:BR47"/>
+    <mergeCell ref="BS47:BV47"/>
+    <mergeCell ref="BW47:BZ47"/>
+    <mergeCell ref="AQ47:AT47"/>
+    <mergeCell ref="AU47:AX47"/>
+    <mergeCell ref="AY47:BB47"/>
+    <mergeCell ref="BC47:BF47"/>
+    <mergeCell ref="BG47:BJ47"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="O47:R47"/>
+    <mergeCell ref="S47:V47"/>
+    <mergeCell ref="W47:Z47"/>
+    <mergeCell ref="AA47:AD47"/>
+    <mergeCell ref="AE47:AH47"/>
+    <mergeCell ref="AI47:AL47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{3202BA62-C7C1-44C7-931A-B83B37570BA9}"/>

</xml_diff>